<commit_message>
Se automatiza el flujo cobro recibo
</commit_message>
<xml_diff>
--- a/Components/SelectTree/Default.xlsx
+++ b/Components/SelectTree/Default.xlsx
@@ -15,12 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>MENU_TREE</t>
   </si>
   <si>
     <t>SUBMENU_TREE</t>
+  </si>
+  <si>
+    <t>SUBMANU2_TREE</t>
   </si>
   <si>
     <t>Acsel;Suscripcion;Emisión / Modificación</t>
@@ -181,30 +184,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="thin">
@@ -218,6 +197,30 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -229,17 +232,17 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -537,34 +540,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="14.96484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="22.60546875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.96484375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22.60546875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" s="6" customFormat="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -581,7 +588,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="8.8984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1"/>

</xml_diff>

<commit_message>
Se crear flujo de siniestros
</commit_message>
<xml_diff>
--- a/Components/SelectTree/Default.xlsx
+++ b/Components/SelectTree/Default.xlsx
@@ -26,10 +26,10 @@
     <t>SUBMANU2_TREE</t>
   </si>
   <si>
-    <t>Acsel;Suscripcion;Emisión / Modificación</t>
+    <t>Acsel;Reclamos</t>
   </si>
   <si>
-    <t>Acsel;Suscripcion</t>
+    <t>Acsel;Reclamos;Siniestros Generales</t>
   </si>
 </sst>
 </file>
@@ -185,7 +185,9 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -194,9 +196,7 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -207,9 +207,7 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -220,7 +218,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -232,18 +232,18 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,7 +543,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -553,11 +553,11 @@
     <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" s="6" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="14.95" s="4" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -565,13 +565,13 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se Crearon scripts de endosos A B D de Autos
</commit_message>
<xml_diff>
--- a/Components/SelectTree/Default.xlsx
+++ b/Components/SelectTree/Default.xlsx
@@ -29,7 +29,7 @@
     <t>Acsel;Reclamos</t>
   </si>
   <si>
-    <t>Acsel;Reclamos;Siniestros Generales</t>
+    <t>Acsel;Suscripcion;Emisión / Modificación</t>
   </si>
 </sst>
 </file>
@@ -185,9 +185,7 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -196,7 +194,9 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -232,18 +232,18 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,35 +543,35 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="14.96484375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="22.60546875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.96484375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22.60546875" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" s="4" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" ht="14.95" s="6" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -588,7 +588,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="16384" width="8.8984375" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="8.8984375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1"/>

</xml_diff>